<commit_message>
Versión final de grupo
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentos/NuevoOrdenDeGrupos.xlsx
+++ b/Sprint 2/Documentos/NuevoOrdenDeGrupos.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Grupo 2" sheetId="2" r:id="rId1"/>
-    <sheet name="Grupo3" sheetId="1" r:id="rId2"/>
+    <sheet name="Grupo 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Grupo 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Grupo3" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Sergio Reyes</t>
   </si>
@@ -86,6 +87,30 @@
   </si>
   <si>
     <t>Alma Negrete(JP)</t>
+  </si>
+  <si>
+    <t>Conocimietos del Grupo 1</t>
+  </si>
+  <si>
+    <t>Arturo Mendoza(JP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alvaro Maldonado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waleska Carreño </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjamin Quintana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felipe Reyes </t>
+  </si>
+  <si>
+    <t>Pedro Becker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pablo Gonzalez </t>
   </si>
 </sst>
 </file>
@@ -139,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -310,8 +335,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,8 +371,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -370,8 +424,12 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="37">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -382,6 +440,14 @@
     <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -392,6 +458,14 @@
     <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,7 +736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,10 +744,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1"/>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="15">
+        <f>AVERAGE(B5:E5)</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" ref="F6:F11" si="0">AVERAGE(B6:E6)</f>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <f>AVERAGE(B9:E9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="22">
+        <v>1</v>
+      </c>
+      <c r="C10" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F10" s="24">
+        <f>AVERAGE(B10:E10)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.45000000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" ref="F13:F15" si="1">AVERAGE(B13:E13)</f>
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="1"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -751,22 +1086,22 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="22">
         <v>0.8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="22">
         <v>0.1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="22">
         <v>0.1</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="23">
         <v>0.8</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="24">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
@@ -856,24 +1191,45 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
+      <c r="A13" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3">
         <v>0.4</v>
       </c>
       <c r="D13" s="3">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E13" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="13">
+        <f>AVERAGE(B13:E13)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" ref="F13:F14" si="1">AVERAGE(B14:E14)</f>
         <v>0.5</v>
-      </c>
-      <c r="F13" s="13">
-        <f t="shared" ref="F13" si="1">AVERAGE(B13:E13)</f>
-        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -887,12 +1243,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -970,22 +1326,22 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="22">
         <v>0.7</v>
       </c>
-      <c r="D7" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="D7" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="24">
         <f t="shared" ref="F7:F11" si="1">AVERAGE(B7:E7)</f>
         <v>0.47499999999999998</v>
       </c>
@@ -1091,8 +1447,29 @@
         <v>1</v>
       </c>
       <c r="F13" s="13">
-        <f t="shared" ref="F13" si="2">AVERAGE(B13:E13)</f>
+        <f t="shared" ref="F13:F14" si="2">AVERAGE(B13:E13)</f>
         <v>0.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="2"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>